<commit_message>
real time data query
</commit_message>
<xml_diff>
--- a/return_all_in.xlsx
+++ b/return_all_in.xlsx
@@ -4,19 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19966" windowHeight="7920"/>
+    <workbookView windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="return" sheetId="1" r:id="rId1"/>
     <sheet name="sharpe ratio" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="sharpe ratio 1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">return!$A$1:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'sharpe ratio 1'!$A$1:$H$27</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+  <si>
+    <t>index</t>
+  </si>
   <si>
     <t>5y</t>
   </si>
@@ -36,6 +44,9 @@
     <t>30y</t>
   </si>
   <si>
+    <t>updated date</t>
+  </si>
+  <si>
     <t>Nasdaq 100</t>
   </si>
   <si>
@@ -51,7 +62,7 @@
     <t>S&amp;P 500</t>
   </si>
   <si>
-    <t>GSPC</t>
+    <t>^HSI</t>
   </si>
   <si>
     <t>SSO</t>
@@ -60,24 +71,56 @@
     <t>UPRO</t>
   </si>
   <si>
+    <t>Dow Jones</t>
+  </si>
+  <si>
+    <t>^DJI</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>^GSPC</t>
+  </si>
+  <si>
     <t>Generally speaking, a Sharpe ratio between 1 and 2 is considered good. A ratio between 2 and 3 is very good, and any result higher than 3 is excellent</t>
   </si>
   <si>
     <t>qld_weight</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>sharpe_ratio</t>
+  </si>
+  <si>
+    <t>median of ratio</t>
+  </si>
+  <si>
+    <t>inverst_duration_years</t>
+  </si>
+  <si>
+    <t>^NDX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??.00_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,27 +129,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.25"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -118,7 +151,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,6 +168,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,7 +190,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -149,30 +198,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -180,14 +206,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,6 +214,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,8 +236,38 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,13 +279,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -275,186 +325,186 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -466,40 +516,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="4"/>
+        <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,7 +556,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,22 +591,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,7 +622,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -584,132 +643,153 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -718,6 +798,7 @@
     <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1039,83 +1120,93 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.95" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.6261682242991" customWidth="1"/>
-    <col min="7" max="7" width="9.5981308411215"/>
+    <col min="1" max="1" width="11.6272727272727" customWidth="1"/>
+    <col min="7" max="7" width="9.6"/>
+    <col min="8" max="8" width="13.0909090909091" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>1.9925</v>
-      </c>
-      <c r="C3" s="7">
-        <v>3.2267</v>
+        <v>1.9873</v>
+      </c>
+      <c r="C3">
+        <v>3.3248</v>
       </c>
       <c r="D3">
-        <v>5.4338</v>
-      </c>
-      <c r="E3" s="7">
-        <v>8.1732</v>
-      </c>
-      <c r="F3" s="8">
-        <v>18.3798</v>
+        <v>5.4508</v>
+      </c>
+      <c r="E3">
+        <v>8.2847</v>
+      </c>
+      <c r="F3">
+        <v>18.2436</v>
       </c>
       <c r="G3">
-        <v>39.2841</v>
+        <v>39.028</v>
+      </c>
+      <c r="H3" s="24">
+        <v>44952</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3.2445</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="25">
         <v>4.8882</v>
       </c>
       <c r="D4">
         <v>8.6618</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="25">
         <v>11.3389</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="26">
         <v>47.525</v>
       </c>
       <c r="G4">
@@ -1124,7 +1215,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4.2605</v>
@@ -1147,35 +1238,38 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>1.4418</v>
+        <v>1.3152</v>
       </c>
       <c r="C7">
-        <v>1.9987</v>
+        <v>1.6302</v>
       </c>
       <c r="D7">
-        <v>2.6733</v>
+        <v>2.319</v>
       </c>
       <c r="E7">
-        <v>3.798</v>
+        <v>2.8995</v>
       </c>
       <c r="F7">
-        <v>5.7374</v>
+        <v>5.5999</v>
       </c>
       <c r="G7">
-        <v>8.0356</v>
+        <v>8.9798</v>
+      </c>
+      <c r="H7" s="24">
+        <v>44952</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1.8691</v>
@@ -1198,7 +1292,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2.0908</v>
@@ -1219,7 +1313,75 @@
         <v>53.3912</v>
       </c>
     </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1.5219</v>
+      </c>
+      <c r="C11">
+        <v>1.8166</v>
+      </c>
+      <c r="D11">
+        <v>2.3237</v>
+      </c>
+      <c r="E11">
+        <v>3.3209</v>
+      </c>
+      <c r="F11">
+        <v>6.2435</v>
+      </c>
+      <c r="G11">
+        <v>10.0048</v>
+      </c>
+      <c r="H11" s="24">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1.4436</v>
+      </c>
+      <c r="C13">
+        <v>2.0064</v>
+      </c>
+      <c r="D13">
+        <v>2.6724</v>
+      </c>
+      <c r="E13">
+        <v>3.8083</v>
+      </c>
+      <c r="F13">
+        <v>5.7181</v>
+      </c>
+      <c r="G13">
+        <v>8.0787</v>
+      </c>
+      <c r="H13" s="24">
+        <v>44952</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H13">
+    <sortState ref="A2:H13">
+      <sortCondition ref="G2" descending="1"/>
+    </sortState>
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1231,109 +1393,109 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79439252336449" defaultRowHeight="13.95" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="8.79090909090909" defaultRowHeight="14.5" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="8.79439252336449" style="1"/>
-    <col min="2" max="2" width="11.803738317757" style="1"/>
-    <col min="3" max="7" width="12.9065420560748" style="1"/>
-    <col min="9" max="9" width="62.9626168224299" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.79090909090909" style="18"/>
+    <col min="2" max="2" width="11.8" style="18"/>
+    <col min="3" max="7" width="12.9090909090909" style="18"/>
+    <col min="9" max="9" width="62.9636363636364" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="18" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="20">
         <v>0.847006560246561</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="20">
         <v>0.942426458694358</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="21">
         <v>1.28826173233342</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="22">
         <v>2.61905694695498</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="23">
         <v>6.55160506818136</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="23">
         <v>4.1149</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="18">
         <v>0.5168</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="18">
         <v>0.4834</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="18">
         <v>0.433</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="18">
         <v>1.3192</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="18">
         <v>3.2459</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="18">
         <v>2.0759</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="18">
         <v>0.3536</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="18">
         <v>0.3412</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="18">
         <v>0.1978</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="18">
         <v>0.489</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="18">
         <v>1.9884</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="18">
         <v>1.3984</v>
       </c>
     </row>
-    <row r="6" ht="41.9" spans="9:9">
-      <c r="I6" s="2" t="s">
-        <v>14</v>
+    <row r="6" ht="29" spans="9:9">
+      <c r="I6" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1348,23 +1510,23 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:C$1048576"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79439252336449" defaultRowHeight="13.95" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.79090909090909" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="11.1308411214953" customWidth="1"/>
+    <col min="1" max="1" width="11.1272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1437,4 +1599,620 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F$1:F$1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="7.72727272727273" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54545454545454" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.1818181818182" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.8181818181818" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.7272727272727" style="3" customWidth="1"/>
+    <col min="8" max="8" width="52.9090909090909" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" hidden="1" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6">
+        <v>9.0273</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5758</v>
+      </c>
+      <c r="D2" s="6">
+        <f>B:B/C:C</f>
+        <v>15.6778395276138</v>
+      </c>
+      <c r="E2" s="6">
+        <v>10.0048</v>
+      </c>
+      <c r="F2" s="7">
+        <v>30</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>89.8619</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50.0967</v>
+      </c>
+      <c r="D3" s="2">
+        <f>B:B/C:C</f>
+        <v>1.79376885104208</v>
+      </c>
+      <c r="E3" s="2">
+        <v>75.6768</v>
+      </c>
+      <c r="F3" s="10">
+        <v>30</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" hidden="1" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7.4249</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.205</v>
+      </c>
+      <c r="D4" s="2">
+        <f>B:B/C:C</f>
+        <v>2.31666146645866</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8.0787</v>
+      </c>
+      <c r="F4" s="11">
+        <v>30</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" hidden="1" spans="1:8">
+      <c r="A5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6">
+        <v>7.7003</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2.4238</v>
+      </c>
+      <c r="D5" s="6">
+        <f>B:B/C:C</f>
+        <v>3.17695354402178</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.9798</v>
+      </c>
+      <c r="F5" s="7">
+        <v>33</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6">
+        <v>39.5608</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9.5084</v>
+      </c>
+      <c r="D6" s="6">
+        <f>B:B/C:C</f>
+        <v>4.16061587648816</v>
+      </c>
+      <c r="E6" s="6">
+        <v>39.028</v>
+      </c>
+      <c r="F6" s="13">
+        <v>30</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>48.4961</v>
+      </c>
+      <c r="C7" s="2">
+        <v>36.313</v>
+      </c>
+      <c r="D7" s="2">
+        <f>B:B/C:C</f>
+        <v>1.33550243714372</v>
+      </c>
+      <c r="E7" s="2">
+        <v>38.6134</v>
+      </c>
+      <c r="F7" s="11">
+        <v>30</v>
+      </c>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>27.0578</v>
+      </c>
+      <c r="C8" s="2">
+        <v>13.5697</v>
+      </c>
+      <c r="D8" s="2">
+        <f>B:B/C:C</f>
+        <v>1.99398660250411</v>
+      </c>
+      <c r="E8" s="2">
+        <v>25.4377</v>
+      </c>
+      <c r="F8" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6">
+        <v>17.0378</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.9603</v>
+      </c>
+      <c r="D9" s="6">
+        <f>B:B/C:C</f>
+        <v>5.75543019288586</v>
+      </c>
+      <c r="E9" s="6">
+        <v>18.2436</v>
+      </c>
+      <c r="F9" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9.6159</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.4754</v>
+      </c>
+      <c r="D10" s="2">
+        <f>B:B/C:C</f>
+        <v>1.48498934428761</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9.2597</v>
+      </c>
+      <c r="F10" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" hidden="1" spans="1:6">
+      <c r="A11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.211</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.0911</v>
+      </c>
+      <c r="D11" s="2">
+        <f>B:B/C:C</f>
+        <v>1.68580764129274</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5.7181</v>
+      </c>
+      <c r="F11" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" hidden="1" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3.3695</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.4815</v>
+      </c>
+      <c r="D12" s="2">
+        <f>B:B/C:C</f>
+        <v>1.35784807576063</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3.8083</v>
+      </c>
+      <c r="F12" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" hidden="1" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.0223</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.632</v>
+      </c>
+      <c r="D13" s="2">
+        <f>B:B/C:C</f>
+        <v>1.23915441176471</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.6724</v>
+      </c>
+      <c r="F13" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" hidden="1" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.0836</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.9156</v>
+      </c>
+      <c r="D14" s="2">
+        <f>B:B/C:C</f>
+        <v>1.18348623853211</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.0064</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" hidden="1" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.4431</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5012</v>
+      </c>
+      <c r="D15" s="2">
+        <f>B:B/C:C</f>
+        <v>0.884078212290503</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.4436</v>
+      </c>
+      <c r="F15" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="6">
+        <v>7.1418</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2.7387</v>
+      </c>
+      <c r="D16" s="6">
+        <f>B:B/C:C</f>
+        <v>2.60773359623179</v>
+      </c>
+      <c r="E16" s="6">
+        <v>8.2847</v>
+      </c>
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <v>8.844</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9.1288</v>
+      </c>
+      <c r="D17" s="2">
+        <f>B:B/C:C</f>
+        <v>0.968802033125931</v>
+      </c>
+      <c r="E17" s="2">
+        <v>7.6645</v>
+      </c>
+      <c r="F17" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4.498</v>
+      </c>
+      <c r="C18" s="2">
+        <v>10.9245</v>
+      </c>
+      <c r="D18" s="2">
+        <f>B:B/C:C</f>
+        <v>0.41173509085084</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.0903</v>
+      </c>
+      <c r="F18" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4.5919</v>
+      </c>
+      <c r="C19" s="6">
+        <v>3.5232</v>
+      </c>
+      <c r="D19" s="6">
+        <f>B:B/C:C</f>
+        <v>1.30333219800182</v>
+      </c>
+      <c r="E19" s="6">
+        <v>5.4508</v>
+      </c>
+      <c r="F19" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7.836</v>
+      </c>
+      <c r="C20" s="2">
+        <v>10.6473</v>
+      </c>
+      <c r="D20" s="2">
+        <f>B:B/C:C</f>
+        <v>0.735961229607506</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5.1918</v>
+      </c>
+      <c r="F20" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2">
+        <v>9.8373</v>
+      </c>
+      <c r="C21" s="2">
+        <v>25.6497</v>
+      </c>
+      <c r="D21" s="2">
+        <f>B:B/C:C</f>
+        <v>0.383524953508228</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2.1221</v>
+      </c>
+      <c r="F21" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2">
+        <v>8.8714</v>
+      </c>
+      <c r="C22" s="2">
+        <v>14.9767</v>
+      </c>
+      <c r="D22" s="2">
+        <f>B:B/C:C</f>
+        <v>0.592346778662856</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.3919</v>
+      </c>
+      <c r="F22" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2">
+        <v>24.6737</v>
+      </c>
+      <c r="C23" s="2">
+        <v>67.2555</v>
+      </c>
+      <c r="D23" s="2">
+        <f>B:B/C:C</f>
+        <v>0.366865163443882</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.9282</v>
+      </c>
+      <c r="F23" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="6">
+        <v>3.3446</v>
+      </c>
+      <c r="C24" s="6">
+        <v>3.5175</v>
+      </c>
+      <c r="D24" s="6">
+        <f>B:B/C:C</f>
+        <v>0.950845771144278</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3.3248</v>
+      </c>
+      <c r="F24" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.0577</v>
+      </c>
+      <c r="C25" s="2">
+        <v>21.3651</v>
+      </c>
+      <c r="D25" s="2">
+        <f>B:B/C:C</f>
+        <v>0.330337793878802</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2.657</v>
+      </c>
+      <c r="F25" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2.9381</v>
+      </c>
+      <c r="C26" s="2">
+        <v>5.7198</v>
+      </c>
+      <c r="D26" s="2">
+        <f>B:B/C:C</f>
+        <v>0.513671806706528</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.3357</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1.1984</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="D27" s="6">
+        <f>B:B/C:C</f>
+        <v>0.849929078014184</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1.9873</v>
+      </c>
+      <c r="F27" s="3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H27">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="TQQQ"/>
+        <filter val="QLD"/>
+        <filter val="^NDX"/>
+      </filters>
+    </filterColumn>
+    <extLst/>
+  </autoFilter>
+  <sortState ref="A2:F27">
+    <sortCondition ref="F2" descending="1"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="H2:H7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>